<commit_message>
updated module path files
</commit_message>
<xml_diff>
--- a/Datasets/UCD_EngArch_Path_Architecture_UG_Modules.xlsx
+++ b/Datasets/UCD_EngArch_Path_Architecture_UG_Modules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\SATLE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBEB9E96-7431-461B-89C9-F42D4C4558CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE02348-1132-4028-8C02-4AAF01E343DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{C7146B4A-4439-46E0-B60E-DB05B9DBCCC1}"/>
   </bookViews>
@@ -508,7 +508,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="I19:J19"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
ARCHITECTURE UG MODULES PATH + CHEM UG MODULES PATH
</commit_message>
<xml_diff>
--- a/Datasets/UCD_EngArch_Path_Architecture_UG_Modules.xlsx
+++ b/Datasets/UCD_EngArch_Path_Architecture_UG_Modules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alanh\Documents\GitHub\ChatGPTAssessment\Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C55FC4-6713-47C8-98A5-231078E6FE79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{680FDCFD-8402-4730-93E7-C9D1D255EF10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C7146B4A-4439-46E0-B60E-DB05B9DBCCC1}"/>
   </bookViews>
@@ -510,7 +510,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17:M26"/>
+      <selection activeCell="G25" sqref="G2:G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>